<commit_message>
Lisää paikkauksen reunoille int-käsittely Excel-tuonnissa
</commit_message>
<xml_diff>
--- a/test/resurssit/excel/urem_tuonti.xlsx
+++ b/test/resurssit/excel/urem_tuonti.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarnova/projects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarnova/projects/harja/test/resurssit/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{580227CD-34F5-E449-91EE-7375D73B6920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626761CE-1C6F-0F42-8459-E779A088967F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47800" yWindow="7760" windowWidth="40040" windowHeight="22460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45340" yWindow="10960" windowWidth="40040" windowHeight="22460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Urapaikkaustoteumien tuonti" sheetId="1" r:id="rId1"/>
@@ -296,22 +296,22 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -697,7 +697,7 @@
   <dimension ref="A1:R235"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -720,24 +720,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
     </row>
     <row r="2" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
@@ -758,10 +758,10 @@
       <c r="P2" s="11"/>
     </row>
     <row r="3" spans="1:18" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
@@ -778,30 +778,30 @@
       <c r="P3" s="11"/>
     </row>
     <row r="4" spans="1:18" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="16">
+      <c r="A4" s="18">
         <v>1.5</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="18" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
       <c r="O4" s="11"/>
       <c r="P4" s="11"/>
     </row>
     <row r="5" spans="1:18" ht="14" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -813,11 +813,11 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="14" t="s">
+      <c r="N5" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
     </row>
     <row r="6" spans="1:18" ht="14" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
@@ -894,10 +894,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" ht="14" x14ac:dyDescent="0.2">
-      <c r="A8" s="20">
+      <c r="A8" s="12">
         <v>43831.416666666701</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="13">
         <v>43831.427083333299</v>
       </c>
       <c r="C8" s="6">
@@ -924,9 +924,15 @@
       <c r="J8" s="6">
         <v>1</v>
       </c>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
+      <c r="K8" s="6">
+        <v>1</v>
+      </c>
+      <c r="L8" s="6">
+        <v>1</v>
+      </c>
+      <c r="M8" s="6">
+        <v>1</v>
+      </c>
       <c r="N8" s="7" t="s">
         <v>24</v>
       </c>
@@ -940,10 +946,10 @@
       <c r="R8" s="6"/>
     </row>
     <row r="9" spans="1:18" ht="14" x14ac:dyDescent="0.2">
-      <c r="A9" s="20">
+      <c r="A9" s="12">
         <v>43831.416666666701</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="13">
         <v>43831.427083333299</v>
       </c>
       <c r="C9" s="6">
@@ -970,9 +976,15 @@
       <c r="J9" s="6">
         <v>1</v>
       </c>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
+      <c r="K9" s="6">
+        <v>2</v>
+      </c>
+      <c r="L9" s="6">
+        <v>2</v>
+      </c>
+      <c r="M9" s="6">
+        <v>1</v>
+      </c>
       <c r="N9" s="7" t="s">
         <v>24</v>
       </c>

</xml_diff>